<commit_message>
Rename Pad to Padding
</commit_message>
<xml_diff>
--- a/media/pre_process.xlsx
+++ b/media/pre_process.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\Manual\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12DDE7C-34B3-4C3A-8C9B-90C73BF6CF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{F12DDE7C-34B3-4C3A-8C9B-90C73BF6CF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AB3026E3-6AC8-43DC-AB9A-1488088598BF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{82FA91C1-AFA3-4631-B311-4F4CA060295C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,47 +38,15 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
+    <t>Pre-processing Type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>GetImage</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pad</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normalize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ResizeTorch</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resize</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CenterCrop</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SetOrder</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resize the input image to the given size using torchvision.transforms.functional.resize.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Resize image tensor to the given size using cv2.resize.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pre-processing Type</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -87,20 +55,51 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Padding</t>
+  </si>
+  <si>
+    <t>Pad image tensor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normalize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normalize image tensor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ResizeTorch</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resize the input image to the given size using torchvision.transforms.functional.resize.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resize</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Resize image tensor to the given size using cv2.resize.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CenterCrop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Center crop the image tensor.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SetOrder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Set the order of axes of the given image tensor.
 Note that this should be at the very end.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Normalize image tensor.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pad image tensor.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Center crop the image tensor.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -108,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -474,77 +473,77 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
     <col min="1" max="1" width="30.625" customWidth="1"/>
     <col min="2" max="2" width="90.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="33">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="B6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="33">
+      <c r="A8" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="33" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>